<commit_message>
Updated Figures for Quantum Journel
</commit_message>
<xml_diff>
--- a/Paper Experiment - Grover/Data - Grover.xlsx
+++ b/Paper Experiment - Grover/Data - Grover.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1996\Google Drive\Lehigh\Research\Jupyter_Code\Paper Experiment - Grover\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1996\Google Drive\Lehigh\Research\Jupyter_Code\Error-Characterization-and-Mitigation\Paper Experiment - Grover\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0424397-7DE5-4B7A-8409-14346FC6E3E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1024A0-8BB4-43EC-A8B6-99041D069B21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11175" yWindow="3900" windowWidth="16410" windowHeight="9465" xr2:uid="{F10DF497-2FBD-41EE-BCB2-5CF4F35E19A3}"/>
+    <workbookView xWindow="13755" yWindow="2415" windowWidth="20730" windowHeight="11835" xr2:uid="{F10DF497-2FBD-41EE-BCB2-5CF4F35E19A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -202,31 +202,31 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -546,7 +546,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +555,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -578,28 +578,28 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
@@ -622,7 +622,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -645,7 +645,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
@@ -668,94 +668,94 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>0.90990000000000004</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>0.93240000000000001</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>0.90629999999999999</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>0.90880000000000005</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>0.92900000000000005</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="5">
         <v>0.91920000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="2">
         <v>0.83779999999999999</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <v>0.86350000000000005</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <v>0.83720000000000006</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
         <v>0.83919999999999995</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="2">
         <v>0.86160000000000003</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="2">
         <v>0.85219999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="8">
         <v>0.91279999999999994</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="8">
         <v>0.93510000000000004</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="8">
         <v>0.90880000000000005</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <v>0.91139999999999999</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="8">
         <v>0.93159999999999998</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="8">
         <v>0.92190000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="2">
         <v>0.89200000000000002</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="2">
         <v>0.91579999999999995</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="2">
         <v>0.89139999999999997</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="2">
         <v>0.89359999999999995</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="2">
         <v>0.91279999999999994</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="2">
         <v>0.90339999999999998</v>
       </c>
     </row>

</xml_diff>